<commit_message>
Reran some of codys old samples
</commit_message>
<xml_diff>
--- a/Thiaminase Activity Assays.12.15.2022/Thiaminase.Assay.Reruns.Key.xlsx
+++ b/Thiaminase Activity Assays.12.15.2022/Thiaminase.Assay.Reruns.Key.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Drew Porter\Thiaminase Activity Assays\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Drew Porter\R\thiaminase\Thiaminase Activity Assays.12.15.2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="12.20.2022.run1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
   <si>
     <t>run2</t>
   </si>
@@ -241,6 +242,72 @@
   </si>
   <si>
     <t>VVB FOSC 03</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 01</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 01</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 02</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 02</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 03</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 03</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 04</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 04</t>
+  </si>
+  <si>
+    <t>12-22 Rainbow Smelt 01</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 05</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 06</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 05</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 07</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 08</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 06</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 07</t>
+  </si>
+  <si>
+    <t>12-22 Rainbow Smelt 02</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 08</t>
+  </si>
+  <si>
+    <t>12-22 Sand Lance 09</t>
+  </si>
+  <si>
+    <t>12-22 Rainbow Smelt 03</t>
+  </si>
+  <si>
+    <t>12-22 Capelin 09</t>
+  </si>
+  <si>
+    <t>12-22 Pacific Herring 01</t>
   </si>
 </sst>
 </file>
@@ -622,7 +689,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E22"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1152,7 @@
   <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,4 +1271,269 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>